<commit_message>
growing season params for toolik added
</commit_message>
<xml_diff>
--- a/ToolikLake/ConfigurationInputsToolik.xlsx
+++ b/ToolikLake/ConfigurationInputsToolik.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Parameter</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>g/m2/yr</t>
+  </si>
+  <si>
+    <t>#ProductionPeriod</t>
+  </si>
+  <si>
+    <t>ProdEndDay</t>
+  </si>
+  <si>
+    <t>ProdStartDay</t>
+  </si>
+  <si>
+    <t>JulianDay</t>
   </si>
 </sst>
 </file>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -541,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>2.9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -552,7 +564,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -719,6 +731,33 @@
       </c>
       <c r="C26" s="3" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>135</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>258</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
param updates for toolik after running optim6
</commit_message>
<xml_diff>
--- a/ToolikLake/ConfigurationInputsToolik.xlsx
+++ b/ToolikLake/ConfigurationInputsToolik.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\SOS\ToolikLake\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="180" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Parameter</t>
   </si>
@@ -139,13 +144,31 @@
   </si>
   <si>
     <t>DOC_sw</t>
+  </si>
+  <si>
+    <t>BurialFactor_R</t>
+  </si>
+  <si>
+    <t>BurialFactor_L</t>
+  </si>
+  <si>
+    <t>POC_lcR</t>
+  </si>
+  <si>
+    <t>POC_lcL</t>
+  </si>
+  <si>
+    <t>DOCR_RespParam</t>
+  </si>
+  <si>
+    <t>DOCL_RespParam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +211,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -236,7 +262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,9 +294,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,6 +329,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,19 +505,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -500,14 +528,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -518,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -529,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -540,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -551,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -562,7 +590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -573,199 +601,265 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>0.01</v>
+        <v>2.0500000000000001E-2</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B14" s="3">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B15" s="3">
         <v>0.13300000000000001</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B18" s="3">
         <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2">
-        <v>6.64</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2">
+        <v>6.64</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B21" s="3">
         <v>2</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B23" s="3">
         <v>0.01</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
+    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B26" s="3">
+        <v>1.66E-2</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3" t="s">
+    <row r="27" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1.66E-2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1.66E-2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B23">
-        <v>0.8</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B29">
+        <v>0.97</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B26">
+      <c r="B32">
         <v>153.36000000000001</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="3" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="3" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B29">
+      <c r="B35">
         <v>135</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B30">
+      <c r="B36">
         <v>258</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -775,24 +869,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>